<commit_message>
add intermeadiate measurements results for Xeon Phi
</commit_message>
<xml_diff>
--- a/Measurements/results/measurements.xlsx
+++ b/Measurements/results/measurements.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="10_7_GPU" sheetId="1" r:id="rId1"/>
     <sheet name="10_7_CPU" sheetId="2" r:id="rId2"/>
+    <sheet name="booster2_CPU" sheetId="3" r:id="rId3"/>
+    <sheet name="booster2_Accelerator" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="19">
   <si>
     <t>naïve</t>
   </si>
@@ -78,6 +80,15 @@
   <si>
     <t xml:space="preserve">Basic </t>
   </si>
+  <si>
+    <t>Intel® Xeon® CPU E5-2660 v2 @ 2.2GHz</t>
+  </si>
+  <si>
+    <t>Intel® Many Integrated Core Acceleration Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic (on CPU) </t>
+  </si>
 </sst>
 </file>
 
@@ -112,8 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -441,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:G53"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,16 +468,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C3" s="1">
@@ -521,7 +535,7 @@
       <c r="X3" s="2"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -582,7 +596,7 @@
       <c r="X4" s="2"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -641,7 +655,7 @@
       <c r="X5" s="2"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -700,7 +714,7 @@
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -759,7 +773,7 @@
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -844,7 +858,7 @@
       <c r="X9" s="2"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="7">
         <v>100</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -905,7 +919,7 @@
       <c r="X10" s="2"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -964,7 +978,7 @@
       <c r="X11" s="2"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1038,7 +1052,7 @@
       <c r="X13" s="2"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="7">
         <v>1000</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1099,7 +1113,7 @@
       <c r="X14" s="2"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1158,7 +1172,7 @@
       <c r="X15" s="2"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1232,7 +1246,7 @@
       <c r="X17" s="2"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="7">
         <v>10000</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1293,7 +1307,7 @@
       <c r="X18" s="2"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1352,7 +1366,7 @@
       <c r="X19" s="2"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1418,7 +1432,7 @@
       <c r="X21" s="2"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="7">
         <v>24</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1479,7 +1493,7 @@
       <c r="X22" s="2"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="5" t="s">
         <v>7</v>
       </c>
@@ -1538,7 +1552,7 @@
       <c r="X23" s="2"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="5" t="s">
         <v>8</v>
       </c>
@@ -1634,7 +1648,7 @@
       <c r="X26" s="2"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+      <c r="A27" s="7">
         <v>100</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1712,7 +1726,7 @@
       <c r="X27" s="2"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="3" t="s">
         <v>1</v>
       </c>
@@ -1788,7 +1802,7 @@
       <c r="X28" s="2"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="3" t="s">
         <v>2</v>
       </c>
@@ -1890,7 +1904,7 @@
       <c r="X30" s="2"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+      <c r="A31" s="7">
         <v>1000</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1968,7 +1982,7 @@
       <c r="X31" s="2"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="3" t="s">
         <v>1</v>
       </c>
@@ -2044,7 +2058,7 @@
       <c r="X32" s="2"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="3" t="s">
         <v>2</v>
       </c>
@@ -2146,7 +2160,7 @@
       <c r="X34" s="2"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
+      <c r="A35" s="7">
         <v>10000</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2200,7 +2214,7 @@
       <c r="X35" s="2"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="3" t="s">
         <v>1</v>
       </c>
@@ -2252,7 +2266,7 @@
       <c r="X36" s="2"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="3" t="s">
         <v>2</v>
       </c>
@@ -2328,7 +2342,7 @@
       <c r="W38" s="2"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2353,15 +2367,15 @@
       <c r="W39" s="2"/>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
+      <c r="A40" s="7"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
@@ -2380,13 +2394,13 @@
       <c r="W40" s="2"/>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+      <c r="A41" s="7"/>
       <c r="B41" s="3"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -2405,132 +2419,132 @@
       <c r="W41" s="2"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
       <c r="W43" s="2"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
       <c r="W44" s="2"/>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
       <c r="W45" s="2"/>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
       <c r="W47" s="2"/>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
       <c r="W48" s="2"/>
     </row>
     <row r="49" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
       <c r="W49" s="2"/>
     </row>
     <row r="50" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
       <c r="W50" s="2"/>
     </row>
     <row r="51" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
       <c r="W51" s="2"/>
     </row>
     <row r="52" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
       <c r="W52" s="2"/>
     </row>
     <row r="53" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2555,8 +2569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,16 +2582,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C3" s="3">
@@ -2630,7 +2644,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -2686,7 +2700,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -2740,7 +2754,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2794,7 +2808,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
@@ -2848,7 +2862,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
@@ -2907,7 +2921,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="7">
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -2963,7 +2977,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
@@ -3017,7 +3031,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
@@ -3071,7 +3085,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="7">
         <v>100</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -3127,7 +3141,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
@@ -3181,7 +3195,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
@@ -3235,7 +3249,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="7">
         <v>1000</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -3291,7 +3305,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
@@ -3345,7 +3359,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
@@ -3409,7 +3423,7 @@
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="7">
         <v>10000</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -3441,7 +3455,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="3" t="s">
         <v>7</v>
       </c>
@@ -3471,7 +3485,7 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
@@ -3509,7 +3523,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+      <c r="A27" s="7">
         <v>4</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -3582,7 +3596,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="3" t="s">
         <v>1</v>
       </c>
@@ -3653,7 +3667,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="3" t="s">
         <v>2</v>
       </c>
@@ -3724,7 +3738,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+      <c r="A31" s="7">
         <v>100</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -3797,7 +3811,7 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="3" t="s">
         <v>1</v>
       </c>
@@ -3868,7 +3882,7 @@
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="3" t="s">
         <v>2</v>
       </c>
@@ -3939,7 +3953,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
+      <c r="A35" s="7">
         <v>1000</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -4012,7 +4026,7 @@
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="3" t="s">
         <v>1</v>
       </c>
@@ -4083,7 +4097,7 @@
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="3" t="s">
         <v>2</v>
       </c>
@@ -4154,7 +4168,7 @@
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
+      <c r="A39" s="7">
         <v>10000</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -4165,7 +4179,7 @@
         <v>14.794386266746059</v>
       </c>
       <c r="D39" s="5">
-        <f t="shared" ref="D39:S39" si="9">D4/D22</f>
+        <f t="shared" ref="D39:J39" si="9">D4/D22</f>
         <v>16.367330055218311</v>
       </c>
       <c r="E39" s="5">
@@ -4203,7 +4217,7 @@
       <c r="S39" s="5"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
+      <c r="A40" s="7"/>
       <c r="B40" s="3" t="s">
         <v>1</v>
       </c>
@@ -4212,7 +4226,7 @@
         <v>10.224799880643372</v>
       </c>
       <c r="D40" s="5">
-        <f t="shared" ref="D40:S40" si="10">D5/D23</f>
+        <f t="shared" ref="D40:J40" si="10">D5/D23</f>
         <v>10.354680467112837</v>
       </c>
       <c r="E40" s="5">
@@ -4250,7 +4264,7 @@
       <c r="S40" s="5"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+      <c r="A41" s="7"/>
       <c r="B41" s="3" t="s">
         <v>2</v>
       </c>
@@ -4288,126 +4302,126 @@
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4426,4 +4440,1522 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C3" s="6">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6">
+        <v>50</v>
+      </c>
+      <c r="E3" s="6">
+        <v>75</v>
+      </c>
+      <c r="F3" s="6">
+        <v>100</v>
+      </c>
+      <c r="G3" s="6">
+        <v>125</v>
+      </c>
+      <c r="H3" s="6">
+        <v>150</v>
+      </c>
+      <c r="I3" s="6">
+        <v>175</v>
+      </c>
+      <c r="J3" s="6">
+        <v>200</v>
+      </c>
+      <c r="L3" s="6">
+        <v>250</v>
+      </c>
+      <c r="M3" s="6">
+        <v>500</v>
+      </c>
+      <c r="N3" s="6">
+        <v>750</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1000</v>
+      </c>
+      <c r="P3" s="6">
+        <v>1250</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>1500</v>
+      </c>
+      <c r="R3" s="6">
+        <v>1750</v>
+      </c>
+      <c r="S3" s="6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5.1910347938500001</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5.2515878677399996</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5.2517530918100004</v>
+      </c>
+      <c r="F4" s="6">
+        <v>5.2809941768600002</v>
+      </c>
+      <c r="G4" s="6">
+        <v>5.2712719440500004</v>
+      </c>
+      <c r="H4" s="6">
+        <v>5.1554200649300004</v>
+      </c>
+      <c r="I4" s="6">
+        <v>5.2332699298899996</v>
+      </c>
+      <c r="J4" s="6">
+        <v>5.2472651004799999</v>
+      </c>
+      <c r="L4" s="6">
+        <v>5.23946285248</v>
+      </c>
+      <c r="M4" s="6">
+        <v>5.2418279647799997</v>
+      </c>
+      <c r="N4" s="6">
+        <v>5.2597489357000002</v>
+      </c>
+      <c r="O4" s="6">
+        <v>5.2307350635500001</v>
+      </c>
+      <c r="P4" s="6">
+        <v>5.2650640010799998</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>5.10460090637</v>
+      </c>
+      <c r="R4" s="6">
+        <v>5.22835707664</v>
+      </c>
+      <c r="S4" s="6">
+        <v>5.1121909618399997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3.48340010643</v>
+      </c>
+      <c r="D5" s="6">
+        <v>3.4994010925299999</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3.5309090614300001</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3.5668938159899999</v>
+      </c>
+      <c r="G5" s="6">
+        <v>3.5491530895199999</v>
+      </c>
+      <c r="H5" s="6">
+        <v>3.4396619796799999</v>
+      </c>
+      <c r="I5" s="6">
+        <v>3.4850199222599998</v>
+      </c>
+      <c r="J5" s="6">
+        <v>3.4936969280199999</v>
+      </c>
+      <c r="L5" s="6">
+        <v>3.5319550037399998</v>
+      </c>
+      <c r="M5" s="6">
+        <v>3.4770460128799998</v>
+      </c>
+      <c r="N5" s="6">
+        <v>3.53223109245</v>
+      </c>
+      <c r="O5" s="6">
+        <v>3.5280718803400002</v>
+      </c>
+      <c r="P5" s="6">
+        <v>3.5504689216599998</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>3.6039049625400001</v>
+      </c>
+      <c r="R5" s="6">
+        <v>3.6270089149500002</v>
+      </c>
+      <c r="S5" s="6">
+        <v>3.6079380512200001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2.0840928554499998</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1.8502128124199999</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2.7882809639000001</v>
+      </c>
+      <c r="F6" s="6">
+        <v>3.24858212471</v>
+      </c>
+      <c r="G6" s="6">
+        <v>2.0671360492700002</v>
+      </c>
+      <c r="H6" s="6">
+        <v>2.3007819652600001</v>
+      </c>
+      <c r="I6" s="6">
+        <v>3.0703270435299999</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1.7045390605899999</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1.4087460040999999</v>
+      </c>
+      <c r="M6" s="6">
+        <v>1.9310970306399999</v>
+      </c>
+      <c r="N6" s="6">
+        <v>2.5553550720199998</v>
+      </c>
+      <c r="O6" s="6">
+        <v>2.4375429153399999</v>
+      </c>
+      <c r="P6" s="6">
+        <v>2.6295881271399999</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>2.5716428756699998</v>
+      </c>
+      <c r="R6" s="6">
+        <v>2.4441277980799998</v>
+      </c>
+      <c r="S6" s="6">
+        <v>3.3674578666700001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>100</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>1000</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.57957100868199996</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.66063690185500001</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.60934090614299996</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.61312699317899999</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.59826302528399999</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.58066201210000001</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.60876917839099998</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0.59729909896900002</v>
+      </c>
+      <c r="L18" s="6">
+        <v>0.67014884948700004</v>
+      </c>
+      <c r="M18" s="6">
+        <v>0.51711916923500001</v>
+      </c>
+      <c r="N18" s="6">
+        <v>0.56043791770899998</v>
+      </c>
+      <c r="O18" s="6">
+        <v>0.69058895111100005</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0.65159201621999996</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>0.59617209434499996</v>
+      </c>
+      <c r="R18" s="6">
+        <v>0.51707792282099996</v>
+      </c>
+      <c r="S18" s="6">
+        <v>0.55800485610999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0.50988316535900002</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.50314784050000005</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.501212835312</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.53807878494299999</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0.62885594367999997</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.48580193519600001</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.50896382331800005</v>
+      </c>
+      <c r="J19" s="6">
+        <v>0.47552490234400002</v>
+      </c>
+      <c r="L19" s="6">
+        <v>0.54447102546699999</v>
+      </c>
+      <c r="M19" s="6">
+        <v>0.53289008140600003</v>
+      </c>
+      <c r="N19" s="6">
+        <v>0.573605060577</v>
+      </c>
+      <c r="O19" s="6">
+        <v>0.52998495101900001</v>
+      </c>
+      <c r="P19" s="6">
+        <v>0.56699299812299997</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>0.55093598365800001</v>
+      </c>
+      <c r="R19" s="6">
+        <v>0.55246210098299997</v>
+      </c>
+      <c r="S19" s="6">
+        <v>0.54261612892199995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>10000</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>4</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>100</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>1000</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="6">
+        <f>C4/C18</f>
+        <v>8.9566847135002678</v>
+      </c>
+      <c r="D35" s="6">
+        <f t="shared" ref="D35:J35" si="0">D4/D18</f>
+        <v>7.9492802369865876</v>
+      </c>
+      <c r="E35" s="6">
+        <f t="shared" si="0"/>
+        <v>8.6187436931692236</v>
+      </c>
+      <c r="F35" s="6">
+        <f t="shared" si="0"/>
+        <v>8.6132142861278904</v>
+      </c>
+      <c r="G35" s="6">
+        <f t="shared" si="0"/>
+        <v>8.8109605997256608</v>
+      </c>
+      <c r="H35" s="6">
+        <f t="shared" si="0"/>
+        <v>8.8785213385754407</v>
+      </c>
+      <c r="I35" s="6">
+        <f t="shared" si="0"/>
+        <v>8.5964764900248909</v>
+      </c>
+      <c r="J35" s="6">
+        <f t="shared" si="0"/>
+        <v>8.7849874703265449</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6">
+        <f>C5/C19</f>
+        <v>6.8317613584621828</v>
+      </c>
+      <c r="D36" s="6">
+        <f t="shared" ref="D36:J36" si="1">D5/D19</f>
+        <v>6.9550156253328872</v>
+      </c>
+      <c r="E36" s="6">
+        <f t="shared" si="1"/>
+        <v>7.0447299284186213</v>
+      </c>
+      <c r="F36" s="6">
+        <f t="shared" si="1"/>
+        <v>6.6289434108944656</v>
+      </c>
+      <c r="G36" s="6">
+        <f t="shared" si="1"/>
+        <v>5.6438253071931275</v>
+      </c>
+      <c r="H36" s="6">
+        <f t="shared" si="1"/>
+        <v>7.080379328444308</v>
+      </c>
+      <c r="I36" s="6">
+        <f t="shared" si="1"/>
+        <v>6.8472841537944893</v>
+      </c>
+      <c r="J36" s="6">
+        <f t="shared" si="1"/>
+        <v>7.3470325335193918</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>10000</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C43" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C43:H57"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A22:A24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C3" s="6">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6">
+        <v>50</v>
+      </c>
+      <c r="E3" s="6">
+        <v>75</v>
+      </c>
+      <c r="F3" s="6">
+        <v>100</v>
+      </c>
+      <c r="G3" s="6">
+        <v>125</v>
+      </c>
+      <c r="H3" s="6">
+        <v>150</v>
+      </c>
+      <c r="I3" s="6">
+        <v>175</v>
+      </c>
+      <c r="J3" s="6">
+        <v>200</v>
+      </c>
+      <c r="L3" s="6">
+        <v>250</v>
+      </c>
+      <c r="M3" s="6">
+        <v>500</v>
+      </c>
+      <c r="N3" s="6">
+        <v>750</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1000</v>
+      </c>
+      <c r="P3" s="6">
+        <v>1250</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>1500</v>
+      </c>
+      <c r="R3" s="6">
+        <v>1750</v>
+      </c>
+      <c r="S3" s="6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5.1910347938500001</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5.2515878677399996</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5.2517530918100004</v>
+      </c>
+      <c r="F4" s="6">
+        <v>5.2809941768600002</v>
+      </c>
+      <c r="G4" s="6">
+        <v>5.2712719440500004</v>
+      </c>
+      <c r="H4" s="6">
+        <v>5.1554200649300004</v>
+      </c>
+      <c r="I4" s="6">
+        <v>5.2332699298899996</v>
+      </c>
+      <c r="J4" s="6">
+        <v>5.2472651004799999</v>
+      </c>
+      <c r="L4" s="6">
+        <v>5.23946285248</v>
+      </c>
+      <c r="M4" s="6">
+        <v>5.2418279647799997</v>
+      </c>
+      <c r="N4" s="6">
+        <v>5.2597489357000002</v>
+      </c>
+      <c r="O4" s="6">
+        <v>5.2307350635500001</v>
+      </c>
+      <c r="P4" s="6">
+        <v>5.2650640010799998</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>5.10460090637</v>
+      </c>
+      <c r="R4" s="6">
+        <v>5.22835707664</v>
+      </c>
+      <c r="S4" s="6">
+        <v>5.1121909618399997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3.48340010643</v>
+      </c>
+      <c r="D5" s="6">
+        <v>3.4994010925299999</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3.5309090614300001</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3.5668938159899999</v>
+      </c>
+      <c r="G5" s="6">
+        <v>3.5491530895199999</v>
+      </c>
+      <c r="H5" s="6">
+        <v>3.4396619796799999</v>
+      </c>
+      <c r="I5" s="6">
+        <v>3.4850199222599998</v>
+      </c>
+      <c r="J5" s="6">
+        <v>3.4936969280199999</v>
+      </c>
+      <c r="L5" s="6">
+        <v>3.5319550037399998</v>
+      </c>
+      <c r="M5" s="6">
+        <v>3.4770460128799998</v>
+      </c>
+      <c r="N5" s="6">
+        <v>3.53223109245</v>
+      </c>
+      <c r="O5" s="6">
+        <v>3.5280718803400002</v>
+      </c>
+      <c r="P5" s="6">
+        <v>3.5504689216599998</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>3.6039049625400001</v>
+      </c>
+      <c r="R5" s="6">
+        <v>3.6270089149500002</v>
+      </c>
+      <c r="S5" s="6">
+        <v>3.6079380512200001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2.0840928554499998</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1.8502128124199999</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2.7882809639000001</v>
+      </c>
+      <c r="F6" s="6">
+        <v>3.24858212471</v>
+      </c>
+      <c r="G6" s="6">
+        <v>2.0671360492700002</v>
+      </c>
+      <c r="H6" s="6">
+        <v>2.3007819652600001</v>
+      </c>
+      <c r="I6" s="6">
+        <v>3.0703270435299999</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1.7045390605899999</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1.4087460040999999</v>
+      </c>
+      <c r="M6" s="6">
+        <v>1.9310970306399999</v>
+      </c>
+      <c r="N6" s="6">
+        <v>2.5553550720199998</v>
+      </c>
+      <c r="O6" s="6">
+        <v>2.4375429153399999</v>
+      </c>
+      <c r="P6" s="6">
+        <v>2.6295881271399999</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>2.5716428756699998</v>
+      </c>
+      <c r="R6" s="6">
+        <v>2.4441277980799998</v>
+      </c>
+      <c r="S6" s="6">
+        <v>3.3674578666700001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>100</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>1000</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="6">
+        <v>4.06010389328</v>
+      </c>
+      <c r="D18" s="6">
+        <v>3.8401958942399999</v>
+      </c>
+      <c r="E18" s="6">
+        <v>3.8402390479999999</v>
+      </c>
+      <c r="F18" s="6">
+        <v>3.73979592323</v>
+      </c>
+      <c r="G18" s="6">
+        <v>4.0413420200300001</v>
+      </c>
+      <c r="H18" s="6">
+        <v>3.9500620365099999</v>
+      </c>
+      <c r="I18" s="6">
+        <v>4.0499939918500001</v>
+      </c>
+      <c r="J18" s="6">
+        <v>4.1098649501800004</v>
+      </c>
+      <c r="L18" s="6">
+        <v>4.01040005684</v>
+      </c>
+      <c r="M18" s="6">
+        <v>4.0102558135999997</v>
+      </c>
+      <c r="N18" s="6">
+        <v>4.0207250118299998</v>
+      </c>
+      <c r="O18" s="6">
+        <v>4.0801479816399997</v>
+      </c>
+      <c r="P18" s="6">
+        <v>4.0798571109799999</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>3.8800837993599999</v>
+      </c>
+      <c r="R18" s="6">
+        <v>3.8798549175299999</v>
+      </c>
+      <c r="S18" s="6">
+        <v>3.8397750854499999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="6">
+        <v>3.9998459816</v>
+      </c>
+      <c r="D19" s="6">
+        <v>4.9001350402800004</v>
+      </c>
+      <c r="E19" s="6">
+        <v>4.0498111247999997</v>
+      </c>
+      <c r="F19" s="6">
+        <v>4.1603400707200002</v>
+      </c>
+      <c r="G19" s="6">
+        <v>4.0295000076300003</v>
+      </c>
+      <c r="H19" s="6">
+        <v>4.0500578880300004</v>
+      </c>
+      <c r="I19" s="6">
+        <v>4.0902938842800003</v>
+      </c>
+      <c r="J19" s="6">
+        <v>4.1002061366999998</v>
+      </c>
+      <c r="L19" s="6">
+        <v>4.0804381370499998</v>
+      </c>
+      <c r="M19" s="6">
+        <v>4.0502779483799998</v>
+      </c>
+      <c r="N19" s="6">
+        <v>4.1199789047199999</v>
+      </c>
+      <c r="O19" s="6">
+        <v>3.80084013939</v>
+      </c>
+      <c r="P19" s="6">
+        <v>3.8388290405299998</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>3.8498508930200002</v>
+      </c>
+      <c r="R19" s="6">
+        <v>4.0500569343599997</v>
+      </c>
+      <c r="S19" s="6">
+        <v>4.1094741821299996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>10000</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>4</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>100</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>1000</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="6">
+        <f>C4/C18</f>
+        <v>1.2785472811279135</v>
+      </c>
+      <c r="D35" s="6">
+        <f t="shared" ref="D35:J35" si="0">D4/D18</f>
+        <v>1.3675312438141449</v>
+      </c>
+      <c r="E35" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3675589009348568</v>
+      </c>
+      <c r="F35" s="6">
+        <f t="shared" si="0"/>
+        <v>1.4121075816080608</v>
+      </c>
+      <c r="G35" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3043370043723421</v>
+      </c>
+      <c r="H35" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3051491387423806</v>
+      </c>
+      <c r="I35" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2921673317099145</v>
+      </c>
+      <c r="J35" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2767487895801015</v>
+      </c>
+      <c r="L35" s="6">
+        <f>L4/L18</f>
+        <v>1.3064688754788323</v>
+      </c>
+      <c r="M35" s="6">
+        <f t="shared" ref="M35:S35" si="1">M4/M18</f>
+        <v>1.3071056332624376</v>
+      </c>
+      <c r="N35" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3081593295299916</v>
+      </c>
+      <c r="O35" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2819964097104946</v>
+      </c>
+      <c r="P35" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2905020587388434</v>
+      </c>
+      <c r="Q35" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3155903764789765</v>
+      </c>
+      <c r="R35" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3475650991528534</v>
+      </c>
+      <c r="S35" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3313777104319326</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6">
+        <f>C5/C19</f>
+        <v>0.87088355963061015</v>
+      </c>
+      <c r="D36" s="6">
+        <f t="shared" ref="D36:J36" si="2">D5/D19</f>
+        <v>0.71414380701027358</v>
+      </c>
+      <c r="E36" s="6">
+        <f t="shared" si="2"/>
+        <v>0.87187005828682307</v>
+      </c>
+      <c r="F36" s="6">
+        <f t="shared" si="2"/>
+        <v>0.85735631110865007</v>
+      </c>
+      <c r="G36" s="6">
+        <f t="shared" si="2"/>
+        <v>0.88079242655405221</v>
+      </c>
+      <c r="H36" s="6">
+        <f t="shared" si="2"/>
+        <v>0.84928711509185251</v>
+      </c>
+      <c r="I36" s="6">
+        <f t="shared" si="2"/>
+        <v>0.85202188910038557</v>
+      </c>
+      <c r="J36" s="6">
+        <f t="shared" si="2"/>
+        <v>0.85207836180447716</v>
+      </c>
+      <c r="L36" s="6">
+        <f>L5/L19</f>
+        <v>0.86558229413409704</v>
+      </c>
+      <c r="M36" s="6">
+        <f t="shared" ref="M36:S36" si="3">M5/M19</f>
+        <v>0.8584709635225708</v>
+      </c>
+      <c r="N36" s="6">
+        <f t="shared" si="3"/>
+        <v>0.85734203357287719</v>
+      </c>
+      <c r="O36" s="6">
+        <f t="shared" si="3"/>
+        <v>0.92823474572814402</v>
+      </c>
+      <c r="P36" s="6">
+        <f t="shared" si="3"/>
+        <v>0.92488331315994521</v>
+      </c>
+      <c r="Q36" s="6">
+        <f t="shared" si="3"/>
+        <v>0.93611546594546968</v>
+      </c>
+      <c r="R36" s="6">
+        <f t="shared" si="3"/>
+        <v>0.89554516732322165</v>
+      </c>
+      <c r="S36" s="6">
+        <f t="shared" si="3"/>
+        <v>0.87795613047262266</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>10000</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C43" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="C43:H57"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A22:A24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>